<commit_message>
Workflow, responsibilities and modules to be created.
</commit_message>
<xml_diff>
--- a/Modules to be implemented.xlsx
+++ b/Modules to be implemented.xlsx
@@ -9,6 +9,9 @@
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Лист1!$A$14:$G$21</definedName>
+  </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
@@ -550,157 +553,157 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1010,7 +1013,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="A14" sqref="A14:G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1024,309 +1027,330 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="44"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="45"/>
     </row>
     <row r="3" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46" t="s">
+      <c r="C3" s="52"/>
+      <c r="D3" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46" t="s">
+      <c r="E3" s="52"/>
+      <c r="F3" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46" t="s">
+      <c r="G3" s="52"/>
+      <c r="H3" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="47"/>
+      <c r="I3" s="53"/>
     </row>
     <row r="4" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="E4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="F4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="G4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="17" t="s">
+      <c r="H4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="25" t="s">
+      <c r="I4" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
-      <c r="B5" s="17" t="s">
+      <c r="A5" s="51"/>
+      <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="17" t="s">
+      <c r="G5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="18"/>
-      <c r="I5" s="26"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="8"/>
     </row>
     <row r="6" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="24"/>
-      <c r="B6" s="17" t="s">
+      <c r="A6" s="51"/>
+      <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="18"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="27"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="10"/>
     </row>
     <row r="7" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="24"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="17" t="s">
+      <c r="A7" s="51"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="E7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="20"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="27"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="10"/>
     </row>
     <row r="8" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="24"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="17" t="s">
+      <c r="A8" s="51"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="E8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="22"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="28"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="12"/>
     </row>
     <row r="9" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30" t="s">
+      <c r="C9" s="48"/>
+      <c r="D9" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="30"/>
-      <c r="F9" s="30" t="s">
+      <c r="E9" s="48"/>
+      <c r="F9" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="G9" s="30"/>
-      <c r="H9" s="30" t="s">
+      <c r="G9" s="48"/>
+      <c r="H9" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="I9" s="31"/>
+      <c r="I9" s="49"/>
     </row>
     <row r="10" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="32"/>
-      <c r="B10" s="33"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="30" t="s">
+      <c r="A10" s="26"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="30"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="30" t="s">
+      <c r="E10" s="48"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="I10" s="31"/>
+      <c r="I10" s="49"/>
     </row>
     <row r="11" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="32"/>
-      <c r="B11" s="35"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="30" t="s">
+      <c r="A11" s="26"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="30"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="36"/>
-      <c r="H11" s="30" t="s">
+      <c r="E11" s="48"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="I11" s="31"/>
+      <c r="I11" s="49"/>
     </row>
     <row r="12" spans="1:9" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="37"/>
-      <c r="B12" s="38"/>
-      <c r="C12" s="39"/>
-      <c r="D12" s="40"/>
-      <c r="E12" s="40"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="40" t="s">
+      <c r="A12" s="27"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="I12" s="41"/>
+      <c r="I12" s="50"/>
     </row>
     <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="48" t="s">
+      <c r="A14" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="49"/>
-      <c r="C14" s="49"/>
-      <c r="D14" s="49"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="49"/>
-      <c r="G14" s="50"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="15"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
     </row>
     <row r="15" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="51" t="s">
+      <c r="A15" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="52" t="s">
+      <c r="B15" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="52"/>
-      <c r="D15" s="52" t="s">
+      <c r="C15" s="39"/>
+      <c r="D15" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="52"/>
-      <c r="F15" s="52" t="s">
+      <c r="E15" s="39"/>
+      <c r="F15" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="G15" s="53"/>
+      <c r="G15" s="41"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4" t="s">
+      <c r="C16" s="40"/>
+      <c r="D16" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4" t="s">
+      <c r="E16" s="40"/>
+      <c r="F16" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="G16" s="5"/>
+      <c r="G16" s="42"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="4" t="s">
+      <c r="A17" s="46"/>
+      <c r="B17" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="8"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="22"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="4" t="s">
+      <c r="A18" s="46"/>
+      <c r="B18" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="11"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="23"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="B19" s="4" t="s">
+      <c r="A19" s="46"/>
+      <c r="B19" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="11"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="23"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="4" t="s">
+      <c r="A20" s="46"/>
+      <c r="B20" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="11"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="23"/>
     </row>
     <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="12"/>
-      <c r="B21" s="13" t="s">
+      <c r="A21" s="47"/>
+      <c r="B21" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="16"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A16:A21"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="A4:A8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
     <mergeCell ref="H5:I8"/>
     <mergeCell ref="A14:G14"/>
     <mergeCell ref="D17:E21"/>
@@ -1343,29 +1367,8 @@
     <mergeCell ref="F15:G15"/>
     <mergeCell ref="F16:G16"/>
     <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A16:A21"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="A4:A8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:I3"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="73" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>